<commit_message>
Saving excel with alters
</commit_message>
<xml_diff>
--- a/excel_scores/titanic.xlsx
+++ b/excel_scores/titanic.xlsx
@@ -444,15 +444,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -461,15 +457,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="B3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -478,15 +470,11 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="5">
@@ -495,15 +483,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -512,15 +496,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -529,15 +509,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="8">
@@ -546,15 +522,11 @@
           <t>C</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="9">
@@ -563,15 +535,11 @@
           <t>B</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="B9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -580,15 +548,11 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="B10" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -597,15 +561,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="12">
@@ -614,15 +574,11 @@
           <t>D</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="13">
@@ -631,15 +587,11 @@
           <t>C</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+      <c r="B13" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="14">
@@ -648,15 +600,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="B14" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="15">
@@ -665,15 +613,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="B15" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="16">
@@ -682,15 +626,11 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
+      <c r="B16" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="17">
@@ -699,15 +639,11 @@
           <t>B</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="B17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -716,15 +652,11 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="B18" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -733,15 +665,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="B19" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -750,15 +678,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="B20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -767,15 +691,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B21" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="22">
@@ -784,15 +704,11 @@
           <t>C</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B22" t="n">
+        <v>5</v>
+      </c>
+      <c r="C22" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="23">
@@ -801,15 +717,11 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="B23" t="n">
+        <v>4</v>
+      </c>
+      <c r="C23" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="24">
@@ -818,15 +730,11 @@
           <t>C</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="B24" t="n">
+        <v>5</v>
+      </c>
+      <c r="C24" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="25">
@@ -835,15 +743,11 @@
           <t>D</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B25" t="n">
+        <v>5</v>
+      </c>
+      <c r="C25" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="26">
@@ -852,15 +756,11 @@
           <t>C</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B26" t="n">
+        <v>5</v>
+      </c>
+      <c r="C26" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="27">
@@ -869,15 +769,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
+      <c r="B27" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="28">
@@ -886,15 +782,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+      <c r="B28" t="n">
+        <v>4</v>
+      </c>
+      <c r="C28" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="29">
@@ -903,15 +795,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="B29" t="n">
+        <v>4</v>
+      </c>
+      <c r="C29" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="30">
@@ -920,15 +808,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B30" t="n">
+        <v>4</v>
+      </c>
+      <c r="C30" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="31">
@@ -937,15 +821,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B31" t="n">
+        <v>4</v>
+      </c>
+      <c r="C31" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="32">
@@ -954,15 +834,11 @@
           <t>E</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B32" t="n">
+        <v>4</v>
+      </c>
+      <c r="C32" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="33">
@@ -971,15 +847,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B33" t="n">
+        <v>4</v>
+      </c>
+      <c r="C33" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="34">
@@ -988,15 +860,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B34" t="n">
+        <v>4</v>
+      </c>
+      <c r="C34" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="35">
@@ -1005,15 +873,11 @@
           <t>E</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B35" t="n">
+        <v>4</v>
+      </c>
+      <c r="C35" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="36">
@@ -1022,15 +886,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B36" t="n">
+        <v>4</v>
+      </c>
+      <c r="C36" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="37">
@@ -1039,15 +899,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B37" t="n">
+        <v>4</v>
+      </c>
+      <c r="C37" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="38">
@@ -1056,15 +912,11 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B38" t="n">
+        <v>4</v>
+      </c>
+      <c r="C38" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="39">
@@ -1073,15 +925,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B39" t="n">
+        <v>4</v>
+      </c>
+      <c r="C39" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="40">
@@ -1090,15 +938,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+      <c r="B40" t="n">
+        <v>4</v>
+      </c>
+      <c r="C40" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="41">
@@ -1107,15 +951,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="B41" t="n">
+        <v>4</v>
+      </c>
+      <c r="C41" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="42">
@@ -1124,15 +964,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B42" t="n">
+        <v>4</v>
+      </c>
+      <c r="C42" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="43">
@@ -1141,15 +977,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B43" t="n">
+        <v>4</v>
+      </c>
+      <c r="C43" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="44">
@@ -1158,15 +990,11 @@
           <t>E</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B44" t="n">
+        <v>4</v>
+      </c>
+      <c r="C44" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="45">
@@ -1175,15 +1003,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B45" t="n">
+        <v>4</v>
+      </c>
+      <c r="C45" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="46">
@@ -1192,15 +1016,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B46" t="n">
+        <v>4</v>
+      </c>
+      <c r="C46" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="47">
@@ -1214,10 +1034,8 @@
           <t>-</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+      <c r="C47" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="48">
@@ -1226,15 +1044,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
+      <c r="B48" t="n">
+        <v>4</v>
+      </c>
+      <c r="C48" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="49">
@@ -1243,15 +1057,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+      <c r="B49" t="n">
+        <v>4</v>
+      </c>
+      <c r="C49" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="50">
@@ -1260,15 +1070,11 @@
           <t>C</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B50" t="n">
+        <v>4</v>
+      </c>
+      <c r="C50" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="51">
@@ -1277,32 +1083,24 @@
           <t>C</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B51" t="n">
+        <v>5</v>
+      </c>
+      <c r="C51" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+          <t>Bb</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>4</v>
+      </c>
+      <c r="C52" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="53">
@@ -1311,15 +1109,11 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B53" t="n">
+        <v>4</v>
+      </c>
+      <c r="C53" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="54">
@@ -1328,15 +1122,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B54" t="n">
+        <v>4</v>
+      </c>
+      <c r="C54" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="55">
@@ -1345,32 +1135,24 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B55" t="n">
+        <v>4</v>
+      </c>
+      <c r="C55" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+          <t>Bb</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>4</v>
+      </c>
+      <c r="C56" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="57">
@@ -1379,15 +1161,11 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B57" t="n">
+        <v>4</v>
+      </c>
+      <c r="C57" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="58">
@@ -1396,15 +1174,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B58" t="n">
+        <v>4</v>
+      </c>
+      <c r="C58" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="59">
@@ -1413,15 +1187,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B59" t="n">
+        <v>4</v>
+      </c>
+      <c r="C59" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="60">
@@ -1430,15 +1200,11 @@
           <t>E</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B60" t="n">
+        <v>4</v>
+      </c>
+      <c r="C60" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="61">
@@ -1447,15 +1213,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B61" t="n">
+        <v>4</v>
+      </c>
+      <c r="C61" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="62">
@@ -1464,15 +1226,11 @@
           <t>E</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B62" t="n">
+        <v>4</v>
+      </c>
+      <c r="C62" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="63">
@@ -1481,15 +1239,11 @@
           <t>D</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
+      <c r="B63" t="n">
+        <v>4</v>
+      </c>
+      <c r="C63" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="64">
@@ -1498,15 +1252,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
+      <c r="B64" t="n">
+        <v>4</v>
+      </c>
+      <c r="C64" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="65">
@@ -1515,15 +1265,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+      <c r="B65" t="n">
+        <v>4</v>
+      </c>
+      <c r="C65" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="66">
@@ -1532,15 +1278,11 @@
           <t>C</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B66" t="n">
+        <v>4</v>
+      </c>
+      <c r="C66" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="67">
@@ -1549,15 +1291,11 @@
           <t>C</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B67" t="n">
+        <v>5</v>
+      </c>
+      <c r="C67" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="68">
@@ -1566,15 +1304,11 @@
           <t>B</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B68" t="n">
+        <v>4</v>
+      </c>
+      <c r="C68" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="69">
@@ -1583,15 +1317,11 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B69" t="n">
+        <v>4</v>
+      </c>
+      <c r="C69" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="70">
@@ -1600,15 +1330,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B70" t="n">
+        <v>4</v>
+      </c>
+      <c r="C70" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="71">
@@ -1617,15 +1343,11 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B71" t="n">
+        <v>4</v>
+      </c>
+      <c r="C71" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="72">
@@ -1634,15 +1356,11 @@
           <t>B</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B72" t="n">
+        <v>4</v>
+      </c>
+      <c r="C72" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="73">
@@ -1651,15 +1369,11 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B73" t="n">
+        <v>4</v>
+      </c>
+      <c r="C73" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="74">
@@ -1668,15 +1382,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B74" t="n">
+        <v>4</v>
+      </c>
+      <c r="C74" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="75">
@@ -1685,15 +1395,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B75" t="n">
+        <v>4</v>
+      </c>
+      <c r="C75" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="76">
@@ -1702,15 +1408,11 @@
           <t>E</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B76" t="n">
+        <v>4</v>
+      </c>
+      <c r="C76" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="77">
@@ -1719,15 +1421,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B77" t="n">
+        <v>4</v>
+      </c>
+      <c r="C77" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="78">
@@ -1736,15 +1434,11 @@
           <t>E</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B78" t="n">
+        <v>4</v>
+      </c>
+      <c r="C78" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="79">
@@ -1753,15 +1447,11 @@
           <t>E</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B79" t="n">
+        <v>4</v>
+      </c>
+      <c r="C79" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="80">
@@ -1770,15 +1460,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B80" t="n">
+        <v>4</v>
+      </c>
+      <c r="C80" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="81">
@@ -1787,15 +1473,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B81" t="n">
+        <v>4</v>
+      </c>
+      <c r="C81" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="82">
@@ -1804,15 +1486,11 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="B82" t="n">
+        <v>4</v>
+      </c>
+      <c r="C82" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="83">
@@ -1821,15 +1499,11 @@
           <t>G</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="B83" t="n">
+        <v>4</v>
+      </c>
+      <c r="C83" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="84">
@@ -1838,15 +1512,11 @@
           <t>F</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
+      <c r="B84" t="n">
+        <v>4</v>
+      </c>
+      <c r="C84" t="n">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creating new logic but still index out of range
</commit_message>
<xml_diff>
--- a/excel_scores/titanic.xlsx
+++ b/excel_scores/titanic.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,6 +434,11 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Chord</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>Duration</t>
         </is>
       </c>
@@ -447,7 +452,10 @@
       <c r="B2" t="n">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
         <v>8</v>
       </c>
     </row>
@@ -460,7 +468,10 @@
       <c r="B3" t="n">
         <v>4</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
         <v>8</v>
       </c>
     </row>
@@ -473,7 +484,10 @@
       <c r="B4" t="n">
         <v>4</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
         <v>48</v>
       </c>
     </row>
@@ -486,7 +500,10 @@
       <c r="B5" t="n">
         <v>4</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
         <v>8</v>
       </c>
     </row>
@@ -499,7 +516,10 @@
       <c r="B6" t="n">
         <v>4</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
         <v>8</v>
       </c>
     </row>
@@ -512,7 +532,10 @@
       <c r="B7" t="n">
         <v>4</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
         <v>16</v>
       </c>
     </row>
@@ -525,7 +548,10 @@
       <c r="B8" t="n">
         <v>5</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
         <v>32</v>
       </c>
     </row>
@@ -538,7 +564,10 @@
       <c r="B9" t="n">
         <v>4</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
         <v>8</v>
       </c>
     </row>
@@ -551,7 +580,10 @@
       <c r="B10" t="n">
         <v>4</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
         <v>8</v>
       </c>
     </row>
@@ -564,7 +596,10 @@
       <c r="B11" t="n">
         <v>4</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
         <v>16</v>
       </c>
     </row>
@@ -577,7 +612,10 @@
       <c r="B12" t="n">
         <v>4</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
         <v>16</v>
       </c>
     </row>
@@ -590,7 +628,10 @@
       <c r="B13" t="n">
         <v>4</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
         <v>24</v>
       </c>
     </row>
@@ -603,7 +644,10 @@
       <c r="B14" t="n">
         <v>4</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
         <v>8</v>
       </c>
     </row>
@@ -616,7 +660,10 @@
       <c r="B15" t="n">
         <v>4</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
         <v>8</v>
       </c>
     </row>
@@ -629,7 +676,10 @@
       <c r="B16" t="n">
         <v>4</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
         <v>48</v>
       </c>
     </row>
@@ -642,7 +692,10 @@
       <c r="B17" t="n">
         <v>4</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
         <v>4</v>
       </c>
     </row>
@@ -655,7 +708,10 @@
       <c r="B18" t="n">
         <v>4</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
         <v>4</v>
       </c>
     </row>
@@ -668,7 +724,10 @@
       <c r="B19" t="n">
         <v>4</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
         <v>4</v>
       </c>
     </row>
@@ -681,7 +740,10 @@
       <c r="B20" t="n">
         <v>4</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
         <v>4</v>
       </c>
     </row>
@@ -694,7 +756,10 @@
       <c r="B21" t="n">
         <v>4</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
         <v>16</v>
       </c>
     </row>
@@ -707,7 +772,10 @@
       <c r="B22" t="n">
         <v>5</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
         <v>32</v>
       </c>
     </row>
@@ -720,7 +788,10 @@
       <c r="B23" t="n">
         <v>4</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
         <v>8</v>
       </c>
     </row>
@@ -733,7 +804,10 @@
       <c r="B24" t="n">
         <v>5</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
         <v>8</v>
       </c>
     </row>
@@ -746,7 +820,10 @@
       <c r="B25" t="n">
         <v>5</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
         <v>16</v>
       </c>
     </row>
@@ -759,7 +836,10 @@
       <c r="B26" t="n">
         <v>5</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
         <v>32</v>
       </c>
     </row>
@@ -772,7 +852,10 @@
       <c r="B27" t="n">
         <v>4</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
         <v>64</v>
       </c>
     </row>
@@ -785,7 +868,10 @@
       <c r="B28" t="n">
         <v>4</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
         <v>24</v>
       </c>
     </row>
@@ -798,7 +884,10 @@
       <c r="B29" t="n">
         <v>4</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
         <v>8</v>
       </c>
     </row>
@@ -811,7 +900,10 @@
       <c r="B30" t="n">
         <v>4</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
         <v>16</v>
       </c>
     </row>
@@ -824,7 +916,10 @@
       <c r="B31" t="n">
         <v>4</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
         <v>16</v>
       </c>
     </row>
@@ -837,7 +932,10 @@
       <c r="B32" t="n">
         <v>4</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
         <v>16</v>
       </c>
     </row>
@@ -850,7 +948,10 @@
       <c r="B33" t="n">
         <v>4</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
         <v>32</v>
       </c>
     </row>
@@ -863,7 +964,10 @@
       <c r="B34" t="n">
         <v>4</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
         <v>16</v>
       </c>
     </row>
@@ -876,7 +980,10 @@
       <c r="B35" t="n">
         <v>4</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
         <v>16</v>
       </c>
     </row>
@@ -889,7 +996,10 @@
       <c r="B36" t="n">
         <v>4</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
         <v>32</v>
       </c>
     </row>
@@ -902,7 +1012,10 @@
       <c r="B37" t="n">
         <v>4</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C37" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
         <v>16</v>
       </c>
     </row>
@@ -915,7 +1028,10 @@
       <c r="B38" t="n">
         <v>4</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
         <v>32</v>
       </c>
     </row>
@@ -928,7 +1044,10 @@
       <c r="B39" t="n">
         <v>4</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
         <v>16</v>
       </c>
     </row>
@@ -941,7 +1060,10 @@
       <c r="B40" t="n">
         <v>4</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
         <v>24</v>
       </c>
     </row>
@@ -954,7 +1076,10 @@
       <c r="B41" t="n">
         <v>4</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C41" t="b">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
         <v>8</v>
       </c>
     </row>
@@ -967,7 +1092,10 @@
       <c r="B42" t="n">
         <v>4</v>
       </c>
-      <c r="C42" t="n">
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
         <v>16</v>
       </c>
     </row>
@@ -980,7 +1108,10 @@
       <c r="B43" t="n">
         <v>4</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C43" t="b">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
         <v>16</v>
       </c>
     </row>
@@ -993,7 +1124,10 @@
       <c r="B44" t="n">
         <v>4</v>
       </c>
-      <c r="C44" t="n">
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1006,7 +1140,10 @@
       <c r="B45" t="n">
         <v>4</v>
       </c>
-      <c r="C45" t="n">
+      <c r="C45" t="b">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
         <v>32</v>
       </c>
     </row>
@@ -1019,7 +1156,10 @@
       <c r="B46" t="n">
         <v>4</v>
       </c>
-      <c r="C46" t="n">
+      <c r="C46" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1034,7 +1174,10 @@
           <t>-</t>
         </is>
       </c>
-      <c r="C47" t="n">
+      <c r="C47" t="b">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1047,7 +1190,10 @@
       <c r="B48" t="n">
         <v>4</v>
       </c>
-      <c r="C48" t="n">
+      <c r="C48" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48" t="n">
         <v>64</v>
       </c>
     </row>
@@ -1060,7 +1206,10 @@
       <c r="B49" t="n">
         <v>4</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C49" t="b">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1073,7 +1222,10 @@
       <c r="B50" t="n">
         <v>4</v>
       </c>
-      <c r="C50" t="n">
+      <c r="C50" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1086,7 +1238,10 @@
       <c r="B51" t="n">
         <v>5</v>
       </c>
-      <c r="C51" t="n">
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
         <v>32</v>
       </c>
     </row>
@@ -1099,7 +1254,10 @@
       <c r="B52" t="n">
         <v>4</v>
       </c>
-      <c r="C52" t="n">
+      <c r="C52" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1112,7 +1270,10 @@
       <c r="B53" t="n">
         <v>4</v>
       </c>
-      <c r="C53" t="n">
+      <c r="C53" t="b">
+        <v>0</v>
+      </c>
+      <c r="D53" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1125,7 +1286,10 @@
       <c r="B54" t="n">
         <v>4</v>
       </c>
-      <c r="C54" t="n">
+      <c r="C54" t="b">
+        <v>0</v>
+      </c>
+      <c r="D54" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1138,7 +1302,10 @@
       <c r="B55" t="n">
         <v>4</v>
       </c>
-      <c r="C55" t="n">
+      <c r="C55" t="b">
+        <v>0</v>
+      </c>
+      <c r="D55" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1151,7 +1318,10 @@
       <c r="B56" t="n">
         <v>4</v>
       </c>
-      <c r="C56" t="n">
+      <c r="C56" t="b">
+        <v>0</v>
+      </c>
+      <c r="D56" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1164,7 +1334,10 @@
       <c r="B57" t="n">
         <v>4</v>
       </c>
-      <c r="C57" t="n">
+      <c r="C57" t="b">
+        <v>0</v>
+      </c>
+      <c r="D57" t="n">
         <v>32</v>
       </c>
     </row>
@@ -1177,7 +1350,10 @@
       <c r="B58" t="n">
         <v>4</v>
       </c>
-      <c r="C58" t="n">
+      <c r="C58" t="b">
+        <v>0</v>
+      </c>
+      <c r="D58" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1190,7 +1366,10 @@
       <c r="B59" t="n">
         <v>4</v>
       </c>
-      <c r="C59" t="n">
+      <c r="C59" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1203,7 +1382,10 @@
       <c r="B60" t="n">
         <v>4</v>
       </c>
-      <c r="C60" t="n">
+      <c r="C60" t="b">
+        <v>0</v>
+      </c>
+      <c r="D60" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1216,7 +1398,10 @@
       <c r="B61" t="n">
         <v>4</v>
       </c>
-      <c r="C61" t="n">
+      <c r="C61" t="b">
+        <v>0</v>
+      </c>
+      <c r="D61" t="n">
         <v>32</v>
       </c>
     </row>
@@ -1229,7 +1414,10 @@
       <c r="B62" t="n">
         <v>4</v>
       </c>
-      <c r="C62" t="n">
+      <c r="C62" t="b">
+        <v>0</v>
+      </c>
+      <c r="D62" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1242,7 +1430,10 @@
       <c r="B63" t="n">
         <v>4</v>
       </c>
-      <c r="C63" t="n">
+      <c r="C63" t="b">
+        <v>0</v>
+      </c>
+      <c r="D63" t="n">
         <v>64</v>
       </c>
     </row>
@@ -1255,7 +1446,10 @@
       <c r="B64" t="n">
         <v>4</v>
       </c>
-      <c r="C64" t="n">
+      <c r="C64" t="b">
+        <v>0</v>
+      </c>
+      <c r="D64" t="n">
         <v>64</v>
       </c>
     </row>
@@ -1268,7 +1462,10 @@
       <c r="B65" t="n">
         <v>4</v>
       </c>
-      <c r="C65" t="n">
+      <c r="C65" t="b">
+        <v>0</v>
+      </c>
+      <c r="D65" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1281,7 +1478,10 @@
       <c r="B66" t="n">
         <v>4</v>
       </c>
-      <c r="C66" t="n">
+      <c r="C66" t="b">
+        <v>0</v>
+      </c>
+      <c r="D66" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1294,7 +1494,10 @@
       <c r="B67" t="n">
         <v>5</v>
       </c>
-      <c r="C67" t="n">
+      <c r="C67" t="b">
+        <v>0</v>
+      </c>
+      <c r="D67" t="n">
         <v>32</v>
       </c>
     </row>
@@ -1307,7 +1510,10 @@
       <c r="B68" t="n">
         <v>4</v>
       </c>
-      <c r="C68" t="n">
+      <c r="C68" t="b">
+        <v>0</v>
+      </c>
+      <c r="D68" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1320,7 +1526,10 @@
       <c r="B69" t="n">
         <v>4</v>
       </c>
-      <c r="C69" t="n">
+      <c r="C69" t="b">
+        <v>0</v>
+      </c>
+      <c r="D69" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1333,7 +1542,10 @@
       <c r="B70" t="n">
         <v>4</v>
       </c>
-      <c r="C70" t="n">
+      <c r="C70" t="b">
+        <v>0</v>
+      </c>
+      <c r="D70" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1346,7 +1558,10 @@
       <c r="B71" t="n">
         <v>4</v>
       </c>
-      <c r="C71" t="n">
+      <c r="C71" t="b">
+        <v>0</v>
+      </c>
+      <c r="D71" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1359,7 +1574,10 @@
       <c r="B72" t="n">
         <v>4</v>
       </c>
-      <c r="C72" t="n">
+      <c r="C72" t="b">
+        <v>0</v>
+      </c>
+      <c r="D72" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1372,7 +1590,10 @@
       <c r="B73" t="n">
         <v>4</v>
       </c>
-      <c r="C73" t="n">
+      <c r="C73" t="b">
+        <v>0</v>
+      </c>
+      <c r="D73" t="n">
         <v>32</v>
       </c>
     </row>
@@ -1385,7 +1606,10 @@
       <c r="B74" t="n">
         <v>4</v>
       </c>
-      <c r="C74" t="n">
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
+      <c r="D74" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1398,7 +1622,10 @@
       <c r="B75" t="n">
         <v>4</v>
       </c>
-      <c r="C75" t="n">
+      <c r="C75" t="b">
+        <v>0</v>
+      </c>
+      <c r="D75" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1411,7 +1638,10 @@
       <c r="B76" t="n">
         <v>4</v>
       </c>
-      <c r="C76" t="n">
+      <c r="C76" t="b">
+        <v>0</v>
+      </c>
+      <c r="D76" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1424,7 +1654,10 @@
       <c r="B77" t="n">
         <v>4</v>
       </c>
-      <c r="C77" t="n">
+      <c r="C77" t="b">
+        <v>0</v>
+      </c>
+      <c r="D77" t="n">
         <v>32</v>
       </c>
     </row>
@@ -1437,7 +1670,10 @@
       <c r="B78" t="n">
         <v>4</v>
       </c>
-      <c r="C78" t="n">
+      <c r="C78" t="b">
+        <v>0</v>
+      </c>
+      <c r="D78" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1450,7 +1686,10 @@
       <c r="B79" t="n">
         <v>4</v>
       </c>
-      <c r="C79" t="n">
+      <c r="C79" t="b">
+        <v>0</v>
+      </c>
+      <c r="D79" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1463,7 +1702,10 @@
       <c r="B80" t="n">
         <v>4</v>
       </c>
-      <c r="C80" t="n">
+      <c r="C80" t="b">
+        <v>0</v>
+      </c>
+      <c r="D80" t="n">
         <v>32</v>
       </c>
     </row>
@@ -1476,7 +1718,10 @@
       <c r="B81" t="n">
         <v>4</v>
       </c>
-      <c r="C81" t="n">
+      <c r="C81" t="b">
+        <v>0</v>
+      </c>
+      <c r="D81" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1489,7 +1734,10 @@
       <c r="B82" t="n">
         <v>4</v>
       </c>
-      <c r="C82" t="n">
+      <c r="C82" t="b">
+        <v>0</v>
+      </c>
+      <c r="D82" t="n">
         <v>32</v>
       </c>
     </row>
@@ -1502,7 +1750,10 @@
       <c r="B83" t="n">
         <v>4</v>
       </c>
-      <c r="C83" t="n">
+      <c r="C83" t="b">
+        <v>0</v>
+      </c>
+      <c r="D83" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1515,7 +1766,10 @@
       <c r="B84" t="n">
         <v>4</v>
       </c>
-      <c r="C84" t="n">
+      <c r="C84" t="b">
+        <v>0</v>
+      </c>
+      <c r="D84" t="n">
         <v>64</v>
       </c>
     </row>

</xml_diff>